<commit_message>
Update to allow Principal Investigators List in grants file
</commit_message>
<xml_diff>
--- a/src/make_cv/files/Proposals & Grants/proposals & grants.xlsx
+++ b/src/make_cv/files/Proposals & Grants/proposals & grants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhelenbr/Codes/make_cv/src/make_cv/files/Proposals &amp; Grants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC57FE07-0E2B-E543-BB44-1C15BF2EF60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F514326-093A-4748-A0D3-C5CB42EDB93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="1500" windowWidth="25800" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>Proposal</t>
   </si>
@@ -31,18 +31,12 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>PCT</t>
   </si>
   <si>
     <t>P_STATUS</t>
   </si>
   <si>
-    <t>Name.1</t>
-  </si>
-  <si>
     <t>Allocated Amt</t>
   </si>
   <si>
@@ -53,12 +47,6 @@
   </si>
   <si>
     <t>Long Descr</t>
-  </si>
-  <si>
-    <t>PRO_BGN_DT</t>
-  </si>
-  <si>
-    <t>PRO_END_DT</t>
   </si>
   <si>
     <t>RO Number</t>
@@ -128,15 +116,6 @@
     <t>2021-09-20</t>
   </si>
   <si>
-    <t>CON0002559</t>
-  </si>
-  <si>
-    <t>Single Crystal Horizontal Growth in Reduced Gravity Environments</t>
-  </si>
-  <si>
-    <t>22194</t>
-  </si>
-  <si>
     <t>CON0003030</t>
   </si>
   <si>
@@ -171,6 +150,39 @@
   </si>
   <si>
     <t>2023-02-08</t>
+  </si>
+  <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>Sponsor</t>
+  </si>
+  <si>
+    <t>Begin Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Principal Investigators</t>
+  </si>
+  <si>
+    <t>Bohl,Douglas Gordon (PI),  Helenbrook,Brian (CPI)</t>
+  </si>
+  <si>
+    <t>Helenbrook,Brian (PI)</t>
+  </si>
+  <si>
+    <t>John. A. Smith and Tom Maiden</t>
+  </si>
+  <si>
+    <t>Erath,Byron D (PI),  Ahmadi,Goodarz (CPI),  Helenbrook,Brian (CPI),  Ferro,Andrea R. (CPI),  Brown,Deborah Martha (CPI)</t>
+  </si>
+  <si>
+    <t>Vu,Tuyen Van (PI),  Ortmeyer,Thomas H. (CPI),  Helenbrook,Brian (CPI)</t>
+  </si>
+  <si>
+    <t>Budisic,Marko (PI),  Helenbrook,Brian (CPI),  Piperni,Pat (CPI)</t>
   </si>
 </sst>
 </file>
@@ -538,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -549,8 +561,8 @@
     <col min="11" max="11" width="57.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -560,45 +572,48 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
+      <c r="P1" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>102239</v>
@@ -607,16 +622,16 @@
         <v>14722</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H2">
         <v>99682.65</v>
@@ -625,10 +640,10 @@
         <v>221517</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L2" s="2">
         <v>44197</v>
@@ -637,15 +652,18 @@
         <v>44926</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="O2" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="P2" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>102526</v>
@@ -654,16 +672,16 @@
         <v>14722</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
       </c>
       <c r="H3">
         <v>8510</v>
@@ -672,10 +690,10 @@
         <v>8510</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L3" s="2">
         <v>44515</v>
@@ -684,15 +702,18 @@
         <v>44607</v>
       </c>
       <c r="N3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="O3" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="P3" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>102466</v>
@@ -701,16 +722,16 @@
         <v>14722</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H4">
         <v>359433.9</v>
@@ -719,10 +740,10 @@
         <v>1996855</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L4" s="2">
         <v>44743</v>
@@ -731,195 +752,163 @@
         <v>46568</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="P4" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5">
-        <v>102563</v>
+        <v>103118</v>
       </c>
       <c r="C5">
         <v>14722</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H5">
-        <v>150000</v>
+        <v>252000</v>
       </c>
       <c r="I5">
-        <v>150000</v>
+        <v>252000</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L5" s="2">
-        <v>44805</v>
+        <v>45505</v>
       </c>
       <c r="M5" s="2">
-        <v>45900</v>
+        <v>46598</v>
       </c>
       <c r="N5" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="O5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6">
-        <v>103118</v>
+        <v>103045</v>
       </c>
       <c r="C6">
         <v>14722</v>
       </c>
       <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
         <v>15</v>
       </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H6">
-        <v>252000</v>
+        <v>149962.79999999999</v>
       </c>
       <c r="I6">
-        <v>252000</v>
+        <v>999752</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="2">
+        <v>45352</v>
+      </c>
+      <c r="M6" s="2">
+        <v>46446</v>
+      </c>
+      <c r="N6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="2">
-        <v>45505</v>
-      </c>
-      <c r="M6" s="2">
-        <v>46598</v>
-      </c>
-      <c r="N6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
       <c r="B7">
-        <v>103045</v>
+        <v>102836</v>
       </c>
       <c r="C7">
         <v>14722</v>
       </c>
       <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
         <v>15</v>
       </c>
-      <c r="E7">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
       <c r="H7">
-        <v>149962.79999999999</v>
+        <v>554124</v>
       </c>
       <c r="I7">
-        <v>999752</v>
+        <v>554124</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L7" s="2">
-        <v>45352</v>
+        <v>45170</v>
       </c>
       <c r="M7" s="2">
-        <v>46446</v>
+        <v>46265</v>
       </c>
       <c r="N7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8">
-        <v>102836</v>
-      </c>
-      <c r="C8">
-        <v>14722</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8">
-        <v>554124</v>
-      </c>
-      <c r="I8">
-        <v>554124</v>
-      </c>
-      <c r="J8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L8" s="2">
-        <v>45170</v>
-      </c>
-      <c r="M8" s="2">
-        <v>46265</v>
-      </c>
-      <c r="N8" t="s">
+        <v>42</v>
+      </c>
+      <c r="P7" t="s">
         <v>48</v>
-      </c>
-      <c r="O8" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to get curve version finalized
</commit_message>
<xml_diff>
--- a/src/make_cv/files/Proposals & Grants/proposals & grants.xlsx
+++ b/src/make_cv/files/Proposals & Grants/proposals & grants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhelenbr/Codes/make_cv/src/make_cv/files/Proposals &amp; Grants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86972211-12DD-9144-B97F-052CEA797902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E7FFDA-F404-C14F-B0F6-8D2625D9A623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1500" windowWidth="42600" windowHeight="19220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="1500" windowWidth="42600" windowHeight="19220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Proposal</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Fields and meanings</t>
+  </si>
+  <si>
+    <t>Proposal_ID</t>
+  </si>
+  <si>
+    <t>Title</t>
   </si>
 </sst>
 </file>
@@ -129,7 +135,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +148,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -179,12 +193,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4283E1CC-4D55-7644-B357-4205C143219F}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -643,92 +658,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="57.83203125" customWidth="1"/>
-    <col min="16" max="16" width="22" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="3" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="57.83203125" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>